<commit_message>
Update PMP & RACI
</commit_message>
<xml_diff>
--- a/PM/RACI-Matrix.xlsx
+++ b/PM/RACI-Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1-ITI\15- Quality Assurance\1- Workshop\1- GIT\GitHub\learning-hub\PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alaa Osama\Documents\GitHub\learning-hub\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E8B5C5-1F90-4BC9-A69B-A10A084D6454}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EA5F17-E870-4D12-8739-47618C2F8202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RACI Matrix Template" sheetId="1" r:id="rId1"/>
@@ -304,7 +304,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -733,19 +733,19 @@
   </sheetPr>
   <dimension ref="A1:UL17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="5.875" customWidth="1"/>
-    <col min="2" max="2" width="51.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" customWidth="1"/>
+    <col min="2" max="2" width="51.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.09765625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="43.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="18.875" customWidth="1"/>
-    <col min="9" max="9" width="22.625" customWidth="1"/>
+    <col min="5" max="5" width="43.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="18.8984375" customWidth="1"/>
+    <col min="9" max="9" width="22.59765625" customWidth="1"/>
     <col min="10" max="11" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -770,7 +770,7 @@
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
     </row>
-    <row r="4" spans="1:558" ht="26.25">
+    <row r="4" spans="1:558" ht="24.6">
       <c r="E4" s="14" t="s">
         <v>13</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="UK5"/>
       <c r="UL5"/>
     </row>
-    <row r="6" spans="1:558" s="2" customFormat="1" ht="24.95" customHeight="1">
+    <row r="6" spans="1:558" s="2" customFormat="1" ht="24.9" customHeight="1">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -1363,20 +1363,20 @@
       <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>2</v>
+      <c r="F6" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>4</v>
@@ -1929,7 +1929,7 @@
       <c r="UK6"/>
       <c r="UL6"/>
     </row>
-    <row r="7" spans="1:558" s="2" customFormat="1" ht="24.95" customHeight="1">
+    <row r="7" spans="1:558" s="2" customFormat="1" ht="24.9" customHeight="1">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -2503,7 +2503,7 @@
       <c r="UK7"/>
       <c r="UL7"/>
     </row>
-    <row r="8" spans="1:558" s="2" customFormat="1" ht="24.95" customHeight="1">
+    <row r="8" spans="1:558" s="2" customFormat="1" ht="24.9" customHeight="1">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -3077,7 +3077,7 @@
       <c r="UK8"/>
       <c r="UL8"/>
     </row>
-    <row r="9" spans="1:558" s="2" customFormat="1" ht="24.95" customHeight="1">
+    <row r="9" spans="1:558" s="2" customFormat="1" ht="24.9" customHeight="1">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
@@ -3651,7 +3651,7 @@
       <c r="UK9"/>
       <c r="UL9"/>
     </row>
-    <row r="10" spans="1:558" s="2" customFormat="1" ht="24.95" customHeight="1">
+    <row r="10" spans="1:558" s="2" customFormat="1" ht="24.9" customHeight="1">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -4225,7 +4225,7 @@
       <c r="UK10"/>
       <c r="UL10"/>
     </row>
-    <row r="11" spans="1:558" s="2" customFormat="1" ht="24.95" customHeight="1">
+    <row r="11" spans="1:558" s="2" customFormat="1" ht="24.9" customHeight="1">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
@@ -4824,7 +4824,7 @@
     <mergeCell ref="E4:K4"/>
     <mergeCell ref="E2:K3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:K1 C4:K10 C2:E2 C3:D3 C12:K168">
+  <conditionalFormatting sqref="C1:K1 C2:E2 C3:D3 C12:K168 C4:K10">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"I"</formula>
     </cfRule>

</xml_diff>